<commit_message>
Corrected X1 PN and PCB's orientation.
</commit_message>
<xml_diff>
--- a/PCB/harp timestamp generator Gen3 BOM.xlsx
+++ b/PCB/harp timestamp generator Gen3 BOM.xlsx
@@ -5,17 +5,28 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OEPS\Google Drive\projects\harp-tech\harp_timestamp_generator Gen3\PCB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OEPS\Documents\github\harp-tech\harp_timestamp_generator_Gen3\PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FF8B6C8-3649-48F3-856E-E6A75B972594}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F49CECE3-4F9C-431E-87BC-858CDCD1527C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="859" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="859" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="harp timestamp generator" sheetId="13" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -234,21 +245,12 @@
     <t>CRCW04021K00FKED</t>
   </si>
   <si>
-    <t>25R</t>
-  </si>
-  <si>
     <t>R2512</t>
   </si>
   <si>
     <t>R15</t>
   </si>
   <si>
-    <t>541-2662-1-ND</t>
-  </si>
-  <si>
-    <t>RCP2512W25R0GEB</t>
-  </si>
-  <si>
     <t>330R</t>
   </si>
   <si>
@@ -351,9 +353,6 @@
     <t>X1</t>
   </si>
   <si>
-    <t>455-1704-ND</t>
-  </si>
-  <si>
     <t>BC817-40LT1SMD</t>
   </si>
   <si>
@@ -721,6 +720,18 @@
   </si>
   <si>
     <t>Farnell</t>
+  </si>
+  <si>
+    <t>15R</t>
+  </si>
+  <si>
+    <t>CRM2512-FX-15R0ELF</t>
+  </si>
+  <si>
+    <t>455-2247-ND</t>
+  </si>
+  <si>
+    <t>B2B-XH-A(LF)(SN)</t>
   </si>
 </sst>
 </file>
@@ -1620,10 +1631,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F50C34B-C9F6-4E1C-A615-C6E180679338}">
-  <dimension ref="A1:H60"/>
+  <dimension ref="A1:I60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C62" sqref="C62"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1681,16 +1692,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>20</v>
@@ -1699,7 +1710,7 @@
         <v>16</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="90" x14ac:dyDescent="0.25">
@@ -1713,7 +1724,7 @@
         <v>4</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>24</v>
@@ -1733,13 +1744,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>45</v>
@@ -1751,7 +1762,7 @@
         <v>16</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1759,16 +1770,16 @@
         <v>1</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>20</v>
@@ -1777,7 +1788,7 @@
         <v>16</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1785,13 +1796,13 @@
         <v>1</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>24</v>
@@ -1817,10 +1828,10 @@
         <v>4</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>20</v>
@@ -1829,7 +1840,7 @@
         <v>16</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1837,16 +1848,16 @@
         <v>2</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>20</v>
@@ -1855,7 +1866,7 @@
         <v>16</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1863,16 +1874,16 @@
         <v>1</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>20</v>
@@ -1881,7 +1892,7 @@
         <v>16</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1889,16 +1900,16 @@
         <v>7</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>20</v>
@@ -1907,7 +1918,7 @@
         <v>16</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1915,7 +1926,7 @@
         <v>1</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>36</v>
@@ -1924,7 +1935,7 @@
         <v>42</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>20</v>
@@ -1933,7 +1944,7 @@
         <v>16</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1941,16 +1952,16 @@
         <v>1</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>20</v>
@@ -1959,7 +1970,7 @@
         <v>16</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1967,16 +1978,16 @@
         <v>3</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>20</v>
@@ -1985,7 +1996,7 @@
         <v>16</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1993,16 +2004,16 @@
         <v>6</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>20</v>
@@ -2011,7 +2022,7 @@
         <v>16</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -2019,16 +2030,16 @@
         <v>1</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>20</v>
@@ -2037,7 +2048,7 @@
         <v>16</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -2045,17 +2056,17 @@
         <v>1</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>129</v>
-      </c>
       <c r="F17" s="4" t="s">
         <v>20</v>
       </c>
@@ -2063,7 +2074,7 @@
         <v>16</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -2071,16 +2082,16 @@
         <v>1</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>20</v>
@@ -2089,7 +2100,7 @@
         <v>16</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -2097,16 +2108,16 @@
         <v>2</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>20</v>
@@ -2115,7 +2126,7 @@
         <v>16</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2123,16 +2134,16 @@
         <v>1</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>20</v>
@@ -2141,7 +2152,7 @@
         <v>16</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2149,16 +2160,16 @@
         <v>3</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>20</v>
@@ -2167,7 +2178,7 @@
         <v>16</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -2175,16 +2186,16 @@
         <v>1</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>20</v>
@@ -2193,7 +2204,7 @@
         <v>16</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2201,17 +2212,17 @@
         <v>5</v>
       </c>
       <c r="B23" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E23" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>91</v>
-      </c>
       <c r="F23" s="4" t="s">
         <v>20</v>
       </c>
@@ -2219,7 +2230,7 @@
         <v>16</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -2227,17 +2238,17 @@
         <v>1</v>
       </c>
       <c r="B24" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="E24" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>150</v>
-      </c>
       <c r="F24" s="4" t="s">
         <v>20</v>
       </c>
@@ -2245,7 +2256,7 @@
         <v>16</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -2253,7 +2264,7 @@
         <v>1</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>31</v>
@@ -2262,7 +2273,7 @@
         <v>32</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>19</v>
@@ -2271,7 +2282,7 @@
         <v>16</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -2279,16 +2290,16 @@
         <v>1</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="F26" s="4" t="s">
         <v>20</v>
@@ -2297,7 +2308,7 @@
         <v>16</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -2305,17 +2316,17 @@
         <v>1</v>
       </c>
       <c r="B27" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E27" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="C27" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>107</v>
-      </c>
       <c r="F27" s="4" t="s">
         <v>20</v>
       </c>
@@ -2323,7 +2334,7 @@
         <v>16</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -2331,17 +2342,17 @@
         <v>1</v>
       </c>
       <c r="B28" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E28" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>102</v>
-      </c>
       <c r="F28" s="4" t="s">
         <v>20</v>
       </c>
@@ -2349,7 +2360,7 @@
         <v>16</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -2357,17 +2368,17 @@
         <v>1</v>
       </c>
       <c r="B29" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E29" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="C29" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>121</v>
-      </c>
       <c r="F29" s="4" t="s">
         <v>20</v>
       </c>
@@ -2375,7 +2386,7 @@
         <v>16</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -2383,17 +2394,17 @@
         <v>1</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C30" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="E30" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="D30" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>122</v>
-      </c>
       <c r="F30" s="4" t="s">
         <v>20</v>
       </c>
@@ -2401,7 +2412,7 @@
         <v>16</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -2418,7 +2429,7 @@
         <v>9</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="F31" s="4" t="s">
         <v>20</v>
@@ -2427,7 +2438,7 @@
         <v>16</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -2456,21 +2467,21 @@
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>3</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F33" s="4" t="s">
         <v>20</v>
@@ -2479,24 +2490,24 @@
         <v>16</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>1</v>
       </c>
       <c r="B34" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="C34" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="D34" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D34" s="3" t="s">
-        <v>60</v>
-      </c>
       <c r="E34" s="3" t="s">
-        <v>62</v>
+        <v>218</v>
       </c>
       <c r="F34" s="4" t="s">
         <v>20</v>
@@ -2505,10 +2516,11 @@
         <v>16</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+      <c r="I34" s="5"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>1</v>
       </c>
@@ -2531,10 +2543,10 @@
         <v>16</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>10</v>
       </c>
@@ -2557,10 +2569,10 @@
         <v>16</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>6</v>
       </c>
@@ -2586,21 +2598,21 @@
         <v>21</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>10</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F38" s="4" t="s">
         <v>20</v>
@@ -2609,24 +2621,24 @@
         <v>16</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>1</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F39" s="4" t="s">
         <v>20</v>
@@ -2635,10 +2647,10 @@
         <v>16</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>1</v>
       </c>
@@ -2664,7 +2676,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>2</v>
       </c>
@@ -2690,7 +2702,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>2</v>
       </c>
@@ -2704,7 +2716,7 @@
         <v>41</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="F42" s="4" t="s">
         <v>20</v>
@@ -2713,10 +2725,10 @@
         <v>16</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>1</v>
       </c>
@@ -2730,7 +2742,7 @@
         <v>34</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="F43" s="4" t="s">
         <v>20</v>
@@ -2739,24 +2751,24 @@
         <v>16</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>1</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="F44" s="4" t="s">
         <v>19</v>
@@ -2765,24 +2777,24 @@
         <v>16</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>10</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="F45" s="4" t="s">
         <v>20</v>
@@ -2791,25 +2803,25 @@
         <v>16</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>1</v>
       </c>
       <c r="B46" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="E46" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="C46" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="E46" s="3" t="s">
-        <v>169</v>
-      </c>
       <c r="F46" s="4" t="s">
         <v>20</v>
       </c>
@@ -2817,24 +2829,24 @@
         <v>16</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>1</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>94</v>
+        <v>220</v>
       </c>
       <c r="F47" s="4" t="s">
         <v>20</v>
@@ -2843,10 +2855,10 @@
         <v>16</v>
       </c>
       <c r="H47" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
         <v>18</v>
       </c>
@@ -2865,10 +2877,10 @@
       <c r="B49"/>
       <c r="C49"/>
       <c r="D49" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="E49" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="F49" s="6"/>
       <c r="G49"/>
@@ -2881,10 +2893,10 @@
       <c r="B50"/>
       <c r="C50"/>
       <c r="D50" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E50" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="F50" s="6"/>
       <c r="G50"/>
@@ -2897,10 +2909,10 @@
       <c r="B51"/>
       <c r="C51"/>
       <c r="D51" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="E51" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="F51" s="6"/>
       <c r="G51"/>
@@ -2913,10 +2925,10 @@
       <c r="B52"/>
       <c r="C52"/>
       <c r="D52" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="E52" s="8" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="F52" s="6"/>
       <c r="G52"/>
@@ -2924,7 +2936,7 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="12" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="B53" s="12"/>
       <c r="C53" s="12"/>
@@ -2941,10 +2953,10 @@
       <c r="B54"/>
       <c r="C54"/>
       <c r="D54" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="E54" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="F54" s="6" t="s">
         <v>17</v>
@@ -2953,7 +2965,7 @@
         <v>16</v>
       </c>
       <c r="H54" s="9" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
@@ -2963,14 +2975,14 @@
       <c r="B55"/>
       <c r="C55"/>
       <c r="D55" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="E55" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="F55" s="6"/>
       <c r="G55" s="7" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="H55" s="9">
         <v>3712278</v>
@@ -2983,13 +2995,13 @@
       <c r="B56"/>
       <c r="C56"/>
       <c r="D56" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="E56" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="H56" s="10">
         <v>3402895</v>

</xml_diff>